<commit_message>
updates for PCBWay assembly order
</commit_message>
<xml_diff>
--- a/PartsOrder.xlsx
+++ b/PartsOrder.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mwg/code/EE Projects 2022-/ESP32-Aorus-Control/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mwg/code/EE Projects 2022-/ESP32-Remote-USB-HID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6B397C-033E-5B4A-8FFE-6BCD2942D40F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0854D7-FBFB-C946-B2FB-F2FFE3962CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="900" yWindow="680" windowWidth="26480" windowHeight="17420" xr2:uid="{7C62EEA5-59C9-AF4A-87E9-63E817F36AD7}"/>
   </bookViews>
@@ -1131,8 +1131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09F5C68B-1182-F246-8D23-02BFEFD1FB78}">
   <dimension ref="A1:S92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>